<commit_message>
Up file 10 cai dau tien nguphapN3 kosei
</commit_message>
<xml_diff>
--- a/NguPhapN3_0724_with_examples.xlsx
+++ b/NguPhapN3_0724_with_examples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dngo30\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\studyingJapanese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64656C50-3869-4822-8CAF-51043A91401C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D070E8FD-0569-4DBB-AC31-86A9736DBEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="364">
   <si>
     <t>～ようになる</t>
   </si>
@@ -1124,6 +1124,129 @@
 → Tự do có nghĩa là có thể hành động theo ý mình.
 「努力」とは、目標のために頑張ることを言います。
 → “Nỗ lực” có nghĩa là cố gắng vì mục tiêu.</t>
+  </si>
+  <si>
+    <t>～うちに</t>
+  </si>
+  <si>
+    <t>Trong lúc
+* Thực hiện một hành động trước khi một trạng thái khác thay đổi
+- 日本にいるうちに一度富士山に登ってみたい。
+Trong lúc còn đang ở Nhật, tôi muốn thử leo núi Phú Sĩ một lần.
+* Trong khoảng thời gian một hành động, sự việc xảy ra, có một trạng thái thay đổi,
+không mang ý chí
+- 音楽を聞いているうちに眠ってしまった。
+ Khi đang nghe nhạc, tôi ngủ thiếp đi mất.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">間 (あいだ) … / ～間に(あいだに)… </t>
+  </si>
+  <si>
+    <t>Trong khoảng thời gian
+* ～間… : Khi một hành động xảy ra trong một thời gian dài, một hành động khác
+cũng xảy ra kéo dài đồng thời trong khoảng thời gian đó
+- お母さんが昼寝をしている間、子どもたちはテレビを見ていた。
+ Trong khi người mẹ đang ngủ trưa thì bọn trẻ ngồi xem tivi.
+* ～間に: Khi một hành động xảy ra trong một thời gian dài, một hành động khác
+xảy ra chỉ tại một thời điểm trong khoảng thời gian đó
+- 私が旅行で留守の間に、庭に草がたくさん生えてしまった。
+ Trong lúc tôi vắng nhà đi du lịch, cỏ dại đã mọc đầy vườn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">～てからでないと… / ～てからでなければ… </t>
+  </si>
+  <si>
+    <t>Nếu không phải là sau khi ～ thì không thể…
+* Cho đến khi việc gì đó được thực hiện xong, thì một việc khác cũng vẫn chưa làm
+được. Câu được dùng ở dạng phủ định
+- 運転免許を取ってからでなければ車を運転してはいけない。
+ Nếu chưa có bằng thì không được phép lái xe.
+- 病気が治ってからでなければ激しい運動は無理だ。
+ Nếu chưa khỏi ốm thì chưa thể vận động mạnh được</t>
+  </si>
+  <si>
+    <t>～ところだ / ～ところ (+trợ từ)</t>
+  </si>
+  <si>
+    <t>Vào thời điểm
+* Khoảnh khắc ngay trước, khoảnh khắc ngay sau, hay vào chính giữa khoảnh khắc
+đó
+- ロケットは間もなく飛び立つところです。緊張の瞬間です。
+ Quả tên lửa chuẩn bị được phóng đi rồi. Khoảnh khắc này thật là hồi hộp.
+- 試験中、となりの人の答えを見ているところを先生に注意された。
+ Trong giờ thi, tôi bị cô giáo nhắc đúng lúc đang nhìn bài bạn bên cạnh</t>
+  </si>
+  <si>
+    <t>N の/ Vる /Vた/・・・＋ ～とおりだ / ～とろり（に）
+N ＋ ～どおりだ /～どおり（に）</t>
+  </si>
+  <si>
+    <t>Dựa theo
+* Thực hiện một hành động giống như hướng dẫn có sẵn, hoặc giống như cách
+người khác làm trước
+- 交番で 教えてもらったとおりに歩いていったので、迷わず会場に着いた。
+ Nhờ đi theo chỉ dẫn của cảnh sát, tôi đã đến được hội trường mà không bị lạc.
+- サッカーの試合の結果はわたしたちの期待どおりだった。
+ Kết quả trận bóng đúng như những gì tôi mong đợi</t>
+  </si>
+  <si>
+    <t>～によって… ～によっては…</t>
+  </si>
+  <si>
+    <t>Tùy vào, tùy theo
+* Thể hiện trạng thái không nhất định mà thay đổi tùy thuộc vào một yếu tố nào
+đó
+- わたしの帰宅時間は毎日違う。日によって 夜中になることもある。
+ Giờ giấc về nhà của tôi mỗi ngày một khác nhau. Tùy hôm, có lúc đêm muộn mới về được.
+- 国によって習慣が違う。
+ Tùy từng nước, tập quán lại khác nhau.</t>
+  </si>
+  <si>
+    <t>N の/ Vる ＋ ～たびに…</t>
+  </si>
+  <si>
+    <t>Mỗi lần
+* Mỗi khi điều gì xảy ra thì có điều khác cũng xảy ra theo. Nhấn mạnh sự lặp lại của
+hành động, nhưng không dùng cho những hiện tượng tự nhiên diễn ra hàng ngày
+- この地方は台風が来るたびに大水の害が起こる。
+ Khu vực này mỗi khi có bão lại phải chịu thiệt hại do ngập lụt.
+- このチームは試合のたびに強くなっていく。
+ Đội (bóng) nay mạnh dần lên sau mỗi trận đấu.</t>
+  </si>
+  <si>
+    <t>（～ば）～ほど /（～なら）～ほど/ ～ほど</t>
+  </si>
+  <si>
+    <t>Càng - càng
+* Phía sau ほど ・・・ là một vế thể hiện sự thay đổi tương ứng, tỉ lệ với vế trước
+- ものが増えれば増えるほど整理が大変になる。
+ Càng nhiều đồ thì việc sắp xếp càng khó hơn.
+- 忙しい人ほど時間の使い方が上手だ。
+ Những người càng bận rộn thì càng giỏi quản lý thời gian hơn.</t>
+  </si>
+  <si>
+    <t>Nの/Vる/Vた + ～ついでに</t>
+  </si>
+  <si>
+    <t>Tiện thể
+* Nhân lúc thực hiện một hành động này thì thì thực hiện thêm một hành động
+khác
+- 散歩のついでにこのはがきをポストに出してきた。
+ Nhân tiện ra ngoài đi dạo, tôi đã đi gửi bưu thiếp.
+- インタネットで本を注文したついでに新しく出たDVDも調べた。
+ Nhân tiện đặt mua sách trên mạng, tôi cũng thử tìm hiểu đĩa DVD mới ra.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N / Vる・ない (Naだ -な) ＋ ～くらい・～ぐらい・～ほど… </t>
+  </si>
+  <si>
+    <t>Tới mức
+* Biểu thị mức độ của một trạng thái sự vật, hiện tượng bằng cách đưa ra một sự vật
+hiện tượng khác
+- 天気予報によると、今日は台風ぐらい風が吹くそうだ。
+ Theo dự báo thời tiết, hôm nay có gió mạnh như bão.
+- さっき地震があった。本棚が倒れるかと思うほど激しく揺れた。
+ Vừa mới có động đất. Mặt đất rung mạnh đến mức tôi tưởng kệ sách bị đổ.</t>
   </si>
 </sst>
 </file>
@@ -1139,12 +1262,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1159,8 +1288,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1465,15 +1598,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34D0AF4-CDA4-493E-881C-BD9EC11D4839}">
-  <dimension ref="A1:B173"/>
+  <dimension ref="A1:B183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.7109375" customWidth="1"/>
+    <col min="2" max="2" width="206.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2860,6 +2994,86 @@
         <v>343</v>
       </c>
     </row>
+    <row r="174" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>346</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>348</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>350</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>354</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>356</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>358</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>360</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>362</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>